<commit_message>
cleaned up some files & updated calendar
</commit_message>
<xml_diff>
--- a/others/Work Calendar-2018.xlsx
+++ b/others/Work Calendar-2018.xlsx
@@ -302,8 +302,8 @@
 3. successfully tested potentiometer</t>
   </si>
   <si>
-    <t>1. motor controller arrives. Test steering
-2. test throttle</t>
+    <t>1. motor controller arrives, updated code
+2. successfully controlled acclerator electonically</t>
   </si>
 </sst>
 </file>
@@ -5142,8 +5142,8 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
recorder added, steering training changes, config stuff added, other small changes
</commit_message>
<xml_diff>
--- a/others/Work Calendar-2018.xlsx
+++ b/others/Work Calendar-2018.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="27840" windowHeight="17080" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full 2018" sheetId="16" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Nov 2018" sheetId="12" r:id="rId12"/>
     <sheet name="Dec 2018" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="85">
   <si>
     <t>SUN</t>
   </si>
@@ -305,11 +305,24 @@
     <t>1. motor controller arrives, updated code
 2. successfully controlled acclerator electonically</t>
   </si>
+  <si>
+    <t>1. Tested the steering on road
+2. Arduino motor control issues fixed
+3. Attempted to do serial commands</t>
+  </si>
+  <si>
+    <t>1. the bug discovered on Friday is gone. (hardware issues?)
+2. tested all components, waiting for testing</t>
+  </si>
+  <si>
+    <t>1. tested the vehicle on public road, didn't work very well. 
+2. debugged Arduino program, attempted to add serial feedback</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -855,7 +868,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -898,7 +917,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -938,6 +963,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -981,7 +1011,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1021,6 +1057,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1064,7 +1105,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1104,6 +1151,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1147,7 +1199,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1190,7 +1248,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1233,7 +1297,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1273,6 +1343,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1316,7 +1391,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1356,6 +1437,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1399,7 +1485,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1439,6 +1531,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1482,7 +1579,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1522,6 +1625,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1565,7 +1673,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1605,6 +1719,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1648,7 +1767,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1688,6 +1813,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1976,8 +2106,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="200" workbookViewId="0">
@@ -4052,8 +4182,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4319,8 +4449,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4591,8 +4721,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet14" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4862,8 +4992,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5138,12 +5268,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5359,11 +5489,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>82</v>
+      </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -5436,8 +5572,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5703,8 +5839,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5981,8 +6117,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6250,8 +6386,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6522,8 +6658,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6793,8 +6929,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -7063,8 +7199,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
segmentation changes but unsucessful
</commit_message>
<xml_diff>
--- a/others/Work Calendar-2018.xlsx
+++ b/others/Work Calendar-2018.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YongyangNie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongyangnie/Developer/ALVNS/others/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17080" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full 2018" sheetId="16" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="Nov 2018" sheetId="12" r:id="rId12"/>
     <sheet name="Dec 2018" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="94">
   <si>
     <t>SUN</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Lincoln's Birthday</t>
-  </si>
-  <si>
-    <t>Ash Wednesday Valentine's Day</t>
   </si>
   <si>
     <t>Vernal Equinox</t>
@@ -329,11 +326,32 @@
     <t xml:space="preserve">1. three successful turns
 2. </t>
   </si>
+  <si>
+    <t>1. really good driving</t>
+  </si>
+  <si>
+    <t>1. good driving</t>
+  </si>
+  <si>
+    <t>1. did some segmentation training</t>
+  </si>
+  <si>
+    <t>1. be able to control the accelerator and breaks</t>
+  </si>
+  <si>
+    <t>1. steering &amp; acceleration &amp; breaking</t>
+  </si>
+  <si>
+    <t>1. make basic decisions about breaking based on segmentation results</t>
+  </si>
+  <si>
+    <t>1. system integration</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -890,6 +908,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -922,27 +961,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,7 +1005,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1030,7 +1054,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1070,6 +1100,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1113,7 +1148,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1153,6 +1194,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1196,7 +1242,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1236,6 +1288,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1279,7 +1336,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1322,7 +1385,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1365,7 +1434,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1405,6 +1480,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1448,7 +1528,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1488,6 +1574,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1531,7 +1622,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1571,6 +1668,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1614,7 +1716,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1654,6 +1762,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1697,7 +1810,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1737,6 +1856,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -1780,7 +1904,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1820,6 +1950,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000003000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -2108,8 +2243,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="200" workbookViewId="0">
@@ -2148,45 +2283,45 @@
       <c r="M1" s="16"/>
     </row>
     <row r="3" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
       <c r="Q3" s="11"/>
-      <c r="R3" s="42" t="s">
+      <c r="R3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
       <c r="Y3" s="11"/>
-      <c r="Z3" s="42" t="s">
+      <c r="Z3" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="10"/>
@@ -2817,45 +2952,45 @@
       <c r="AF10" s="5"/>
     </row>
     <row r="12" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="42" t="s">
+      <c r="J12" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
       <c r="Q12" s="11"/>
-      <c r="R12" s="42" t="s">
+      <c r="R12" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="42"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
       <c r="Y12" s="11"/>
-      <c r="Z12" s="42" t="s">
+      <c r="Z12" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="AA12" s="42"/>
-      <c r="AB12" s="42"/>
-      <c r="AC12" s="42"/>
-      <c r="AD12" s="42"/>
-      <c r="AE12" s="42"/>
-      <c r="AF12" s="42"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
     </row>
     <row r="13" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
@@ -3490,45 +3625,45 @@
       <c r="AF19" s="5"/>
     </row>
     <row r="21" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="42" t="s">
+      <c r="J21" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
       <c r="Q21" s="11"/>
-      <c r="R21" s="42" t="s">
+      <c r="R21" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="42"/>
-      <c r="W21" s="42"/>
-      <c r="X21" s="42"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="49"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="49"/>
       <c r="Y21" s="11"/>
-      <c r="Z21" s="42" t="s">
+      <c r="Z21" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AA21" s="42"/>
-      <c r="AB21" s="42"/>
-      <c r="AC21" s="42"/>
-      <c r="AD21" s="42"/>
-      <c r="AE21" s="42"/>
-      <c r="AF21" s="42"/>
+      <c r="AA21" s="49"/>
+      <c r="AB21" s="49"/>
+      <c r="AC21" s="49"/>
+      <c r="AD21" s="49"/>
+      <c r="AE21" s="49"/>
+      <c r="AF21" s="49"/>
     </row>
     <row r="22" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
@@ -4184,8 +4319,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4201,15 +4336,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -4417,23 +4552,23 @@
         <f>H11+1</f>
         <v>30</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="24"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4451,8 +4586,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4468,15 +4603,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -4688,24 +4823,24 @@
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4723,8 +4858,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet14" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -4740,15 +4875,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -4959,24 +5094,24 @@
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4994,8 +5129,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -5011,15 +5146,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -5179,7 +5314,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="9"/>
     </row>
@@ -5235,24 +5370,24 @@
         <f>B13+1</f>
         <v>31</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5270,12 +5405,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5287,15 +5422,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -5353,16 +5488,16 @@
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5398,22 +5533,22 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="E6" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="F6" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="G6" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="24" t="s">
         <v>76</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5449,19 +5584,19 @@
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="24"/>
       <c r="C8" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>80</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="H8" s="24"/>
     </row>
@@ -5497,20 +5632,20 @@
     </row>
     <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="E10" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="F10" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>85</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>86</v>
       </c>
       <c r="H10" s="24"/>
     </row>
@@ -5519,41 +5654,45 @@
         <f>H9+1</f>
         <v>28</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
     </row>
     <row r="12" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="24"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>87</v>
+      </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="47"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5571,12 +5710,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5588,15 +5727,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -5638,7 +5777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -5679,13 +5818,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="C6" s="24" t="s">
+        <v>89</v>
+      </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5718,17 +5861,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D8" s="24"/>
-      <c r="E8" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="E8" s="9"/>
       <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="24" t="s">
+        <v>92</v>
+      </c>
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5761,7 +5904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="9" t="s">
         <v>17</v>
@@ -5769,7 +5912,9 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>93</v>
+      </c>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5797,30 +5942,32 @@
       <c r="B12" s="24"/>
       <c r="C12" s="39"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="35"/>
+      <c r="E12" s="35" t="s">
+        <v>91</v>
+      </c>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5838,12 +5985,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5855,15 +6002,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -6030,7 +6177,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
@@ -6077,28 +6224,28 @@
         <v>19</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -6116,8 +6263,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6133,15 +6280,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -6197,7 +6344,7 @@
     </row>
     <row r="4" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -6319,7 +6466,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -6350,24 +6497,24 @@
       <c r="H12" s="34"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -6385,8 +6532,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6402,15 +6549,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -6622,24 +6769,24 @@
       <c r="H12" s="33"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -6657,8 +6804,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6674,15 +6821,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -6805,7 +6952,7 @@
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
@@ -6848,7 +6995,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -6893,24 +7040,24 @@
       <c r="H12" s="36"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -6928,8 +7075,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6945,15 +7092,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -7163,24 +7310,24 @@
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -7198,8 +7345,8 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -7215,15 +7362,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
@@ -7431,24 +7578,24 @@
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
latest changes to be pushed to cart
</commit_message>
<xml_diff>
--- a/others/Work Calendar-2018.xlsx
+++ b/others/Work Calendar-2018.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="96">
   <si>
     <t>SUN</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>1. system integration</t>
+  </si>
+  <si>
+    <t>1. trained more segmentation stuff. The software is mostly working</t>
+  </si>
+  <si>
+    <t>1. training and software engineering</t>
   </si>
 </sst>
 </file>
@@ -5715,7 +5721,7 @@
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5824,11 +5830,13 @@
         <v>89</v>
       </c>
       <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24" t="s">
-        <v>90</v>
-      </c>
+      <c r="E6" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="24"/>
       <c r="H6" s="24"/>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5868,7 +5876,9 @@
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="24"/>
+      <c r="F8" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="G8" s="24" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
arduino code updated, ready for some testing
</commit_message>
<xml_diff>
--- a/others/Work Calendar-2018.xlsx
+++ b/others/Work Calendar-2018.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="96">
   <si>
     <t>SUN</t>
   </si>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>2018 FULL YEAR CALENDAR TEMPLATE</t>
-  </si>
-  <si>
-    <t>Lincoln's Birthday</t>
   </si>
   <si>
     <t>Vernal Equinox</t>
@@ -336,22 +333,25 @@
     <t>1. did some segmentation training</t>
   </si>
   <si>
-    <t>1. be able to control the accelerator and breaks</t>
-  </si>
-  <si>
-    <t>1. steering &amp; acceleration &amp; breaking</t>
-  </si>
-  <si>
-    <t>1. make basic decisions about breaking based on segmentation results</t>
-  </si>
-  <si>
-    <t>1. system integration</t>
-  </si>
-  <si>
     <t>1. trained more segmentation stuff. The software is mostly working</t>
   </si>
   <si>
     <t>1. training and software engineering</t>
+  </si>
+  <si>
+    <t>1. able to stop vehicle when encounters obstacle (off road testing)</t>
+  </si>
+  <si>
+    <t>1. able to stop when encounters obstacle (on road testing). However, break motor too weak</t>
+  </si>
+  <si>
+    <t>1. be able to make basic decision with segmentation results</t>
+  </si>
+  <si>
+    <t>1. on road auto cruise control system testing</t>
+  </si>
+  <si>
+    <t>1. on road whole system testing</t>
   </si>
 </sst>
 </file>
@@ -5320,7 +5320,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="9"/>
     </row>
@@ -5494,16 +5494,16 @@
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5539,22 +5539,22 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="E6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="F6" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="G6" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="24" t="s">
         <v>75</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5590,19 +5590,19 @@
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="24"/>
       <c r="C8" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>79</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="H8" s="24"/>
     </row>
@@ -5639,19 +5639,19 @@
     <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="E10" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="F10" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>84</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>85</v>
       </c>
       <c r="H10" s="24"/>
     </row>
@@ -5671,10 +5671,10 @@
       <c r="B12" s="24"/>
       <c r="C12" s="43"/>
       <c r="D12" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
@@ -5720,8 +5720,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="176" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5827,14 +5827,14 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -5872,13 +5872,13 @@
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="D8" s="24"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="24" t="s">
-        <v>90</v>
-      </c>
+      <c r="E8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="24"/>
       <c r="G8" s="24" t="s">
         <v>92</v>
       </c>
@@ -5919,12 +5919,14 @@
       <c r="C10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>94</v>
+      </c>
       <c r="F10" s="24"/>
-      <c r="G10" s="24" t="s">
-        <v>93</v>
-      </c>
+      <c r="G10" s="24"/>
       <c r="H10" s="24"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5953,7 +5955,7 @@
       <c r="C12" s="39"/>
       <c r="D12" s="40"/>
       <c r="E12" s="35" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
@@ -6187,7 +6189,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
@@ -6234,7 +6236,7 @@
         <v>19</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -6354,7 +6356,7 @@
     </row>
     <row r="4" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -6476,7 +6478,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -6962,7 +6964,7 @@
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
@@ -7005,7 +7007,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>

</xml_diff>

<commit_message>
lots of small training changes
tried to improve the steering system but didn't really
</commit_message>
<xml_diff>
--- a/others/Work Calendar-2018.xlsx
+++ b/others/Work Calendar-2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17080" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27840" windowHeight="17080" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full 2018" sheetId="16" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="99">
   <si>
     <t>SUN</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Groundhog Day</t>
-  </si>
-  <si>
-    <t>President's Day</t>
   </si>
   <si>
     <t>St Patrick's Day</t>
@@ -330,28 +327,42 @@
     <t>1. good driving</t>
   </si>
   <si>
-    <t>1. did some segmentation training</t>
-  </si>
-  <si>
     <t>1. trained more segmentation stuff. The software is mostly working</t>
   </si>
   <si>
     <t>1. training and software engineering</t>
   </si>
   <si>
-    <t>1. able to stop vehicle when encounters obstacle (off road testing)</t>
-  </si>
-  <si>
     <t>1. able to stop when encounters obstacle (on road testing). However, break motor too weak</t>
   </si>
   <si>
     <t>1. be able to make basic decision with segmentation results</t>
   </si>
   <si>
-    <t>1. on road auto cruise control system testing</t>
-  </si>
-  <si>
     <t>1. on road whole system testing</t>
+  </si>
+  <si>
+    <t>1. finished the new braking system</t>
+  </si>
+  <si>
+    <t>1. install new motor controller &amp; test out whole entire system</t>
+  </si>
+  <si>
+    <t>1. debug test results from Wednesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. on road auto cruise control system testing
+2. work with new GPS </t>
+  </si>
+  <si>
+    <t>1. engineered the brake motor system</t>
+  </si>
+  <si>
+    <t>1. able to stop vehicle when encounters obstacle (off road testing)
+2. realized some flaws in the hardware</t>
+  </si>
+  <si>
+    <t>1. segmentation training</t>
   </si>
 </sst>
 </file>
@@ -2274,7 +2285,7 @@
     <row r="1" spans="1:39" s="17" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="14"/>
@@ -2290,7 +2301,7 @@
     </row>
     <row r="3" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
@@ -2300,7 +2311,7 @@
       <c r="H3" s="49"/>
       <c r="I3" s="11"/>
       <c r="J3" s="49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="49"/>
       <c r="L3" s="49"/>
@@ -2310,7 +2321,7 @@
       <c r="P3" s="49"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S3" s="49"/>
       <c r="T3" s="49"/>
@@ -2320,7 +2331,7 @@
       <c r="X3" s="49"/>
       <c r="Y3" s="11"/>
       <c r="Z3" s="49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AA3" s="49"/>
       <c r="AB3" s="49"/>
@@ -2959,7 +2970,7 @@
     </row>
     <row r="12" spans="1:39" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="49"/>
       <c r="D12" s="49"/>
@@ -2969,7 +2980,7 @@
       <c r="H12" s="49"/>
       <c r="I12" s="11"/>
       <c r="J12" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
@@ -2979,7 +2990,7 @@
       <c r="P12" s="49"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S12" s="49"/>
       <c r="T12" s="49"/>
@@ -2989,7 +3000,7 @@
       <c r="X12" s="49"/>
       <c r="Y12" s="11"/>
       <c r="Z12" s="49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA12" s="49"/>
       <c r="AB12" s="49"/>
@@ -3632,7 +3643,7 @@
     </row>
     <row r="21" spans="2:32" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="49"/>
@@ -3642,7 +3653,7 @@
       <c r="H21" s="49"/>
       <c r="I21" s="11"/>
       <c r="J21" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K21" s="49"/>
       <c r="L21" s="49"/>
@@ -3652,7 +3663,7 @@
       <c r="P21" s="49"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S21" s="49"/>
       <c r="T21" s="49"/>
@@ -3662,7 +3673,7 @@
       <c r="X21" s="49"/>
       <c r="Y21" s="11"/>
       <c r="Z21" s="49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AA21" s="49"/>
       <c r="AB21" s="49"/>
@@ -4343,7 +4354,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -4428,7 +4439,7 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24"/>
       <c r="C6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -4610,7 +4621,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -4710,7 +4721,7 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24"/>
       <c r="C6" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
@@ -4822,7 +4833,7 @@
       <c r="C12" s="26"/>
       <c r="D12" s="27"/>
       <c r="E12" s="41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="23"/>
@@ -4882,7 +4893,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -4972,7 +4983,7 @@
     </row>
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="9"/>
@@ -5013,7 +5024,7 @@
     </row>
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -5058,7 +5069,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -5153,7 +5164,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -5320,7 +5331,7 @@
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="9"/>
     </row>
@@ -5357,10 +5368,10 @@
     <row r="12" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
@@ -5387,7 +5398,7 @@
     <row r="14" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="57"/>
       <c r="E14" s="58"/>
@@ -5415,7 +5426,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="135" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="135" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -5429,7 +5440,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -5494,16 +5505,16 @@
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="G4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -5539,22 +5550,22 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="E6" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="F6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="G6" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="H6" s="24" t="s">
         <v>74</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -5590,19 +5601,19 @@
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="24"/>
       <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>78</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>79</v>
       </c>
       <c r="H8" s="24"/>
     </row>
@@ -5639,19 +5650,19 @@
     <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="E10" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="F10" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>83</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="H10" s="24"/>
     </row>
@@ -5671,10 +5682,10 @@
       <c r="B12" s="24"/>
       <c r="C12" s="43"/>
       <c r="D12" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
@@ -5720,8 +5731,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="176" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" zoomScale="176" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5734,7 +5745,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -5827,14 +5838,16 @@
     <row r="6" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24" t="s">
-        <v>90</v>
-      </c>
       <c r="F6" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -5872,15 +5885,17 @@
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="24"/>
+        <v>90</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>96</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H8" s="24"/>
     </row>
@@ -5917,15 +5932,17 @@
     <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="9" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D10" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="24"/>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
     </row>
@@ -5955,7 +5972,7 @@
       <c r="C12" s="39"/>
       <c r="D12" s="40"/>
       <c r="E12" s="35" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
@@ -6015,7 +6032,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6144,7 +6161,7 @@
     </row>
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -6152,7 +6169,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="24"/>
       <c r="H8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -6189,7 +6206,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
@@ -6233,10 +6250,10 @@
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
       <c r="G12" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:8" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -6293,7 +6310,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6356,7 +6373,7 @@
     </row>
     <row r="4" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -6478,7 +6495,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="24"/>
       <c r="G10" s="24"/>
@@ -6562,7 +6579,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6697,7 +6714,7 @@
     </row>
     <row r="8" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -6772,7 +6789,7 @@
     <row r="12" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="24"/>
       <c r="C12" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
@@ -6834,7 +6851,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -6964,7 +6981,7 @@
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
@@ -7001,13 +7018,13 @@
     </row>
     <row r="10" spans="2:8" ht="56" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -7105,7 +7122,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -7171,7 +7188,7 @@
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
@@ -7375,7 +7392,7 @@
   <sheetData>
     <row r="1" spans="2:8" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>

</xml_diff>